<commit_message>
GoodInfo_v2 - 2021.11.24 完成
</commit_message>
<xml_diff>
--- a/GoodInfo_StockList_20211124_drop.xlsx
+++ b/GoodInfo_StockList_20211124_drop.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
@@ -536,33 +536,37 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>1712</v>
+        <v>2484</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>興農</t>
+          <t>希華</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G3" t="n">
         <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>1.3</v>
+        <v>1.86</v>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>3.84</v>
+      </c>
       <c r="K3" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="L3" t="inlineStr"/>
+        <v>1.86</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.4843750000000001</v>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>right_only</t>
@@ -571,36 +575,36 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>2484</v>
+        <v>5351</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>希華</t>
+          <t>鈺創</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G4" t="n">
         <v>3</v>
       </c>
       <c r="H4" t="n">
-        <v>1.86</v>
+        <v>0.7</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
-        <v>3.84</v>
+        <v>1.1</v>
       </c>
       <c r="K4" t="n">
-        <v>1.86</v>
+        <v>0.7</v>
       </c>
       <c r="L4" t="n">
-        <v>0.4843750000000001</v>
+        <v>0.6363636363636362</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -610,36 +614,36 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>5351</v>
+        <v>6265</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>鈺創</t>
+          <t>方土昶</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G5" t="n">
         <v>3</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
-        <v>1.1</v>
+        <v>2.76</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6363636363636362</v>
+        <v>0.2717391304347826</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -649,37 +653,35 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>6265</v>
+        <v>6568</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>方土昶</t>
+          <t>宏觀</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G6" t="n">
         <v>3</v>
       </c>
       <c r="H6" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="n">
-        <v>2.76</v>
-      </c>
+        <v>2.12</v>
+      </c>
+      <c r="I6" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.2717391304347826</v>
-      </c>
+        <v>13.82</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
           <t>right_only</t>
@@ -688,35 +690,37 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>6568</v>
+        <v>3041</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>宏觀</t>
+          <t>揚智</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="H7" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="I7" t="n">
-        <v>11.7</v>
-      </c>
-      <c r="J7" t="inlineStr"/>
+        <v>22.8</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>16.25</v>
+      </c>
       <c r="K7" t="n">
-        <v>13.82</v>
-      </c>
-      <c r="L7" t="inlineStr"/>
+        <v>22.8</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.403076923076923</v>
+      </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>right_only</t>
@@ -725,36 +729,38 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>3041</v>
+        <v>3122</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>揚智</t>
+          <t>笙泉</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G8" t="n">
         <v>2.9</v>
       </c>
       <c r="H8" t="n">
-        <v>22.8</v>
-      </c>
-      <c r="I8" t="inlineStr"/>
+        <v>3.2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>9.140000000000001</v>
+      </c>
       <c r="J8" t="n">
-        <v>16.25</v>
+        <v>12.34</v>
       </c>
       <c r="K8" t="n">
-        <v>22.8</v>
+        <v>12.34</v>
       </c>
       <c r="L8" t="n">
-        <v>1.403076923076923</v>
+        <v>1</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -764,39 +770,35 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>3122</v>
+        <v>3221</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>笙泉</t>
+          <t>台嘉碩</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G9" t="n">
         <v>2.9</v>
       </c>
       <c r="H9" t="n">
-        <v>3.2</v>
+        <v>7.84</v>
       </c>
       <c r="I9" t="n">
-        <v>9.140000000000001</v>
-      </c>
-      <c r="J9" t="n">
-        <v>12.34</v>
-      </c>
+        <v>3.8</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
-        <v>12.34</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1</v>
-      </c>
+        <v>11.64</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
           <t>right_only</t>
@@ -805,35 +807,39 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>3221</v>
+        <v>3515</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>台嘉碩</t>
+          <t>華擎</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G10" t="n">
         <v>2.9</v>
       </c>
       <c r="H10" t="n">
-        <v>7.84</v>
+        <v>4.24</v>
       </c>
       <c r="I10" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>11.24</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4.17</v>
+      </c>
       <c r="K10" t="n">
-        <v>11.64</v>
-      </c>
-      <c r="L10" t="inlineStr"/>
+        <v>15.48</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3.712230215827338</v>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>right_only</t>
@@ -842,38 +848,38 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>3515</v>
+        <v>3588</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>華擎</t>
+          <t>通嘉</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G11" t="n">
         <v>2.9</v>
       </c>
       <c r="H11" t="n">
-        <v>4.24</v>
+        <v>3.22</v>
       </c>
       <c r="I11" t="n">
-        <v>11.24</v>
+        <v>5.96</v>
       </c>
       <c r="J11" t="n">
-        <v>4.17</v>
+        <v>8.18</v>
       </c>
       <c r="K11" t="n">
-        <v>15.48</v>
+        <v>9.18</v>
       </c>
       <c r="L11" t="n">
-        <v>3.712230215827338</v>
+        <v>1.122249388753056</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -883,38 +889,36 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="n">
-        <v>3588</v>
+        <v>5371</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>通嘉</t>
+          <t>中光電</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G12" t="n">
         <v>2.9</v>
       </c>
       <c r="H12" t="n">
-        <v>3.22</v>
-      </c>
-      <c r="I12" t="n">
-        <v>5.96</v>
-      </c>
+        <v>17.58</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="n">
-        <v>8.18</v>
+        <v>11.37</v>
       </c>
       <c r="K12" t="n">
-        <v>9.18</v>
+        <v>17.58</v>
       </c>
       <c r="L12" t="n">
-        <v>1.122249388753056</v>
+        <v>1.546174142480211</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -924,37 +928,35 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>5371</v>
+        <v>6411</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>中光電</t>
+          <t>晶焱</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G13" t="n">
         <v>2.9</v>
       </c>
       <c r="H13" t="n">
-        <v>17.58</v>
-      </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="n">
-        <v>11.37</v>
-      </c>
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5.92</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>17.58</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1.546174142480211</v>
-      </c>
+        <v>6.48</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
           <t>right_only</t>
@@ -963,33 +965,33 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>6411</v>
+        <v>8040</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>晶焱</t>
+          <t>九暘</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G14" t="n">
         <v>2.9</v>
       </c>
       <c r="H14" t="n">
-        <v>0.5600000000000001</v>
+        <v>7.96</v>
       </c>
       <c r="I14" t="n">
-        <v>5.92</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
-        <v>6.48</v>
+        <v>17.16</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
@@ -1000,33 +1002,31 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="n">
-        <v>8040</v>
+        <v>1110</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>九暘</t>
+          <t>東泥</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="H15" t="n">
-        <v>7.96</v>
-      </c>
-      <c r="I15" t="n">
-        <v>9.199999999999999</v>
-      </c>
+        <v>4.46</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
-        <v>17.16</v>
+        <v>4.46</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
@@ -1037,31 +1037,29 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="n">
-        <v>1110</v>
+        <v>2338</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>東泥</t>
+          <t>光罩</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
+        <v>6</v>
+      </c>
+      <c r="G16" t="n">
         <v>2</v>
       </c>
-      <c r="G16" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H16" t="n">
-        <v>4.46</v>
-      </c>
+      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
-        <v>4.46</v>
+        <v>0</v>
       </c>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
@@ -1072,20 +1070,20 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="n">
-        <v>2338</v>
+        <v>3455</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>光罩</t>
+          <t>由田</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="G17" t="n">
         <v>2</v>
@@ -1105,20 +1103,20 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="n">
-        <v>3312</v>
+        <v>5258</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>弘憶股</t>
+          <t>虹堡</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G18" t="n">
         <v>2</v>
@@ -1138,20 +1136,20 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="n">
-        <v>3455</v>
+        <v>5347</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>由田</t>
+          <t>世界</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G19" t="n">
         <v>2</v>
@@ -1171,20 +1169,20 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="n">
-        <v>5258</v>
+        <v>6143</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>虹堡</t>
+          <t>振曜</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G20" t="n">
         <v>2</v>
@@ -1204,20 +1202,20 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="n">
-        <v>5347</v>
+        <v>6285</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>世界</t>
+          <t>啟碁</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="G21" t="n">
         <v>2</v>
@@ -1237,20 +1235,20 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="n">
-        <v>6143</v>
+        <v>6438</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>振曜</t>
+          <t>迅得</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G22" t="n">
         <v>2</v>
@@ -1270,20 +1268,20 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
-        <v>6285</v>
+        <v>8054</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>啟碁</t>
+          <t>安國</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G23" t="n">
         <v>2</v>
@@ -1303,20 +1301,20 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="n">
-        <v>6438</v>
+        <v>8112</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>迅得</t>
+          <t>至上</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G24" t="n">
         <v>2</v>
@@ -1334,72 +1332,6 @@
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="n">
-        <v>8054</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>安國</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>59</v>
-      </c>
-      <c r="G25" t="n">
-        <v>2</v>
-      </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>right_only</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>8112</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>至上</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="n">
-        <v>62</v>
-      </c>
-      <c r="G26" t="n">
-        <v>2</v>
-      </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>right_only</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>